<commit_message>
added N=29:35 into shell distribution excel list Started to write a script for macro values fixed a couple of mistakes in cluster2.1.R file (there were a couple! grrr)
</commit_message>
<xml_diff>
--- a/R working directory/Results/Распределение частиц по оболочкам.xlsx
+++ b/R working directory/Results/Распределение частиц по оболочкам.xlsx
@@ -437,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,6 +782,72 @@
       </c>
       <c r="C30" s="1">
         <v>103.7366</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2">
+        <v>6.24</v>
+      </c>
+      <c r="C31" s="1">
+        <v>109.193</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="2">
+        <v>5.26</v>
+      </c>
+      <c r="C32" s="1">
+        <v>115.1801</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="2">
+        <v>6.26</v>
+      </c>
+      <c r="C33" s="1">
+        <v>120.8746</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="2">
+        <v>6.27</v>
+      </c>
+      <c r="C34" s="1">
+        <v>126.6955</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="2">
+        <v>6.28</v>
+      </c>
+      <c r="C35" s="1">
+        <v>132.71549999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="2">
+        <v>7.28</v>
+      </c>
+      <c r="C36" s="1">
+        <v>139.41759999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>